<commit_message>
Add a 3rd UART
</commit_message>
<xml_diff>
--- a/hardware/expansion_board_V0/Conception.xlsx
+++ b/hardware/expansion_board_V0/Conception.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="0" windowWidth="27705" windowHeight="13020"/>
+    <workbookView xWindow="7665" yWindow="0" windowWidth="27705" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="239">
   <si>
     <t>TTL</t>
   </si>
@@ -733,13 +732,22 @@
   </si>
   <si>
     <t>LV_MUXB</t>
+  </si>
+  <si>
+    <t>Uart3</t>
+  </si>
+  <si>
+    <t>RX3</t>
+  </si>
+  <si>
+    <t>TX3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -800,13 +808,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -925,10 +945,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1016,23 +1037,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutre" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1311,11 +1336,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V159"/>
+  <dimension ref="A1:V161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S91" sqref="S91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2055,14 +2080,14 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42"/>
-      <c r="C42" s="36"/>
+      <c r="C42" s="34"/>
       <c r="E42" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43"/>
-      <c r="C43" s="36"/>
+      <c r="C43" s="34"/>
       <c r="E43" s="12" t="s">
         <v>21</v>
       </c>
@@ -2081,14 +2106,14 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44"/>
-      <c r="C44" s="36"/>
+      <c r="C44" s="34"/>
       <c r="E44" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45"/>
-      <c r="C45" s="33" t="s">
+      <c r="C45" s="35" t="s">
         <v>24</v>
       </c>
       <c r="E45" s="5" t="s">
@@ -2109,7 +2134,7 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46"/>
-      <c r="C46" s="34"/>
+      <c r="C46" s="36"/>
       <c r="E46" s="7" t="s">
         <v>5</v>
       </c>
@@ -2145,13 +2170,13 @@
       </c>
     </row>
     <row r="49" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="36"/>
+      <c r="C49" s="34"/>
       <c r="E49" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C50" s="36"/>
+      <c r="C50" s="34"/>
       <c r="E50" s="12" t="s">
         <v>21</v>
       </c>
@@ -2172,13 +2197,13 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C51" s="36"/>
+      <c r="C51" s="34"/>
       <c r="E51" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C52" s="33" t="s">
+      <c r="C52" s="35" t="s">
         <v>24</v>
       </c>
       <c r="E52" s="5" t="s">
@@ -2198,7 +2223,7 @@
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C53" s="34"/>
+      <c r="C53" s="36"/>
       <c r="E53" s="7" t="s">
         <v>5</v>
       </c>
@@ -2676,7 +2701,7 @@
       </c>
     </row>
     <row r="80" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>64</v>
       </c>
@@ -2696,7 +2721,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>64</v>
       </c>
@@ -2716,7 +2741,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>64</v>
       </c>
@@ -2736,7 +2761,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>64</v>
       </c>
@@ -2756,7 +2781,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>64</v>
       </c>
@@ -2776,7 +2801,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>64</v>
       </c>
@@ -2796,7 +2821,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>64</v>
       </c>
@@ -2816,7 +2841,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>64</v>
       </c>
@@ -2836,19 +2861,17 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>64</v>
-      </c>
+    <row r="89" spans="1:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A90" s="38"/>
       <c r="C90" s="5" t="s">
-        <v>98</v>
+        <v>236</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>190</v>
+        <v>237</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>74</v>
@@ -2856,15 +2879,17 @@
       <c r="K90">
         <v>1</v>
       </c>
-      <c r="R90" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C91" s="11"/>
-      <c r="E91" s="11"/>
+      <c r="S90" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C91" s="13"/>
+      <c r="E91" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="I91" s="2" t="s">
-        <v>191</v>
+        <v>238</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>75</v>
@@ -2873,65 +2898,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C92" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E92" s="11"/>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="I92" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="K92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="R92" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C93" s="11"/>
       <c r="E93" s="11"/>
       <c r="I93" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J93" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K93">
         <v>1</v>
       </c>
-      <c r="R93" s="9">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C94" s="13"/>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C94" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="E94" s="11"/>
       <c r="I94" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="K94">
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E95" s="11"/>
       <c r="I95" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>74</v>
@@ -2943,13 +2970,11 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C96" s="13"/>
-      <c r="E96" s="7" t="s">
-        <v>73</v>
-      </c>
+      <c r="E96" s="11"/>
       <c r="I96" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>75</v>
@@ -2958,383 +2983,391 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E97" s="11"/>
+      <c r="I97" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="J97" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K97">
+        <v>1</v>
+      </c>
+      <c r="R97" s="9">
+        <v>0.2</v>
+      </c>
+    </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C98" s="5" t="s">
+      <c r="C98" s="13"/>
+      <c r="E98" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C100" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E98" s="5" t="s">
+      <c r="E100" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I98" s="2" t="s">
+      <c r="I100" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="J98" s="2" t="s">
+      <c r="J100" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="K98">
-        <v>1</v>
-      </c>
-      <c r="R98" s="9">
+      <c r="K100">
+        <v>1</v>
+      </c>
+      <c r="R100" s="9">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C99" s="11"/>
-      <c r="E99" s="11"/>
-      <c r="I99" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="J99" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C100" s="11"/>
-      <c r="E100" s="11"/>
-      <c r="I100" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="J100" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="K100">
-        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C101" s="11"/>
       <c r="E101" s="11"/>
       <c r="I101" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="K101">
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C102" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="C102" s="11"/>
       <c r="E102" s="11"/>
       <c r="I102" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K102">
         <v>1</v>
-      </c>
-      <c r="R102" s="9">
-        <v>0.1</v>
       </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C103" s="11"/>
       <c r="E103" s="11"/>
       <c r="I103" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J103" s="2" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="K103">
         <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C104" s="11"/>
+      <c r="A104" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E104" s="11"/>
       <c r="I104" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K104">
+        <v>1</v>
+      </c>
+      <c r="R104" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C105" s="11"/>
+      <c r="E105" s="11"/>
+      <c r="I105" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C106" s="11"/>
+      <c r="E106" s="11"/>
+      <c r="I106" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="J104" s="2" t="s">
+      <c r="J106" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="K104">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C105" s="13"/>
-      <c r="E105" s="7" t="s">
+      <c r="K106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C107" s="13"/>
+      <c r="E107" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="I105" s="2" t="s">
+      <c r="I107" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="J105" s="2" t="s">
+      <c r="J107" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K105">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>64</v>
-      </c>
-      <c r="C107" s="5" t="s">
+      <c r="K107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>64</v>
+      </c>
+      <c r="C109" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E107" s="5" t="s">
+      <c r="E109" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I107" s="2" t="s">
+      <c r="I109" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="J107" s="2" t="s">
+      <c r="J109" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="K107">
-        <v>1</v>
-      </c>
-      <c r="R107" s="9">
+      <c r="K109">
+        <v>1</v>
+      </c>
+      <c r="R109" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A108"/>
-      <c r="C108" s="11"/>
-      <c r="E108" s="11"/>
-      <c r="I108" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="K108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A109"/>
-      <c r="C109" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E109" s="11"/>
-      <c r="I109" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="J109" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K109">
-        <v>1</v>
-      </c>
-    </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>64</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="A110"/>
+      <c r="C110" s="11"/>
       <c r="E110" s="11"/>
       <c r="I110" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J110" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K110">
         <v>1</v>
-      </c>
-      <c r="R110" s="9">
-        <v>0.1</v>
       </c>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111"/>
-      <c r="C111" s="11"/>
+      <c r="C111" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="E111" s="11"/>
       <c r="I111" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="J111" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>64</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E112" s="11"/>
+      <c r="I112" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K112">
+        <v>1</v>
+      </c>
+      <c r="R112" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A113"/>
+      <c r="C113" s="11"/>
+      <c r="E113" s="11"/>
+      <c r="I113" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="J111" s="2" t="s">
+      <c r="J113" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="K111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C112" s="7" t="s">
+      <c r="K113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C114" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E112" s="7" t="s">
+      <c r="E114" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="I112" s="2" t="s">
+      <c r="I114" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="J112" s="2" t="s">
+      <c r="J114" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C114" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="E114" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="N114">
-        <v>1</v>
-      </c>
-      <c r="P114" s="19"/>
-      <c r="Q114" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="R114" s="19"/>
-    </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C115" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="E115" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="N115">
-        <v>1</v>
-      </c>
-      <c r="Q115" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="R115" s="19"/>
-    </row>
+      <c r="K114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="E116" s="15"/>
+        <v>94</v>
+      </c>
+      <c r="E116" s="15" t="s">
+        <v>79</v>
+      </c>
       <c r="N116">
         <v>1</v>
       </c>
-      <c r="R116" s="9">
-        <v>0.3</v>
-      </c>
+      <c r="P116" s="19"/>
+      <c r="Q116" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="R116" s="19"/>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C117" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E117" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="N117">
+        <v>1</v>
+      </c>
+      <c r="Q117" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="R117" s="19"/>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C118" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E118" s="15"/>
+      <c r="N118">
+        <v>1</v>
+      </c>
+      <c r="R118" s="9">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C119" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E117" s="15"/>
-      <c r="N117">
-        <v>1</v>
-      </c>
-      <c r="R117" s="9">
+      <c r="E119" s="15"/>
+      <c r="N119">
+        <v>1</v>
+      </c>
+      <c r="R119" s="9">
         <v>0.3</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C118" s="29" t="s">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C120" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="E118" s="15"/>
-    </row>
-    <row r="119" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C119" s="3"/>
-      <c r="E119" s="3"/>
-    </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C120" s="5" t="s">
+      <c r="E120" s="15"/>
+    </row>
+    <row r="121" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C121" s="3"/>
+      <c r="E121" s="3"/>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C122" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E120" s="4"/>
-    </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C121" s="12" t="s">
+      <c r="E122" s="4"/>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C123" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E121" s="5" t="s">
+      <c r="E123" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I121" s="2" t="s">
+      <c r="I123" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="J121" s="2" t="s">
+      <c r="J123" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="K121">
-        <v>1</v>
-      </c>
-      <c r="L121">
+      <c r="K123">
+        <v>1</v>
+      </c>
+      <c r="L123">
         <v>-8</v>
       </c>
-      <c r="R121" s="31">
+      <c r="R123" s="31">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C122" s="12"/>
-      <c r="E122" s="11"/>
-      <c r="I122" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="J122" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="K122">
-        <v>1</v>
-      </c>
-      <c r="R122" s="31"/>
-    </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C123" s="12"/>
-      <c r="E123" s="11"/>
-      <c r="I123" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="J123" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="K123">
-        <v>1</v>
-      </c>
-      <c r="R123" s="31"/>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C124" s="12"/>
       <c r="E124" s="11"/>
       <c r="I124" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J124" s="2" t="s">
-        <v>212</v>
+        <v>78</v>
       </c>
       <c r="K124">
         <v>1</v>
@@ -3343,81 +3376,81 @@
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C125" s="12"/>
-      <c r="E125" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="E125" s="11"/>
       <c r="I125" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J125" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="K125">
         <v>1</v>
       </c>
+      <c r="R125" s="31"/>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C126" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E126" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="C126" s="12"/>
+      <c r="E126" s="11"/>
       <c r="I126" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="J126" s="2" t="s">
-        <v>77</v>
+        <v>212</v>
       </c>
       <c r="K126">
         <v>1</v>
       </c>
-      <c r="M126">
-        <v>-16</v>
-      </c>
-      <c r="R126" s="31">
-        <v>0.08</v>
-      </c>
+      <c r="R126" s="31"/>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C127" s="12"/>
-      <c r="E127" s="11"/>
+      <c r="E127" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="I127" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J127" s="2" t="s">
-        <v>76</v>
+        <v>211</v>
       </c>
       <c r="K127">
         <v>1</v>
       </c>
-      <c r="R127" s="31"/>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C128" s="12"/>
-      <c r="E128" s="11"/>
+      <c r="A128" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C128" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="I128" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J128" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K128">
         <v>1</v>
       </c>
-      <c r="R128" s="31"/>
+      <c r="M128">
+        <v>-16</v>
+      </c>
+      <c r="R128" s="31">
+        <v>0.08</v>
+      </c>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C129" s="12"/>
       <c r="E129" s="11"/>
       <c r="I129" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J129" s="2" t="s">
-        <v>215</v>
+        <v>76</v>
       </c>
       <c r="K129">
         <v>1</v>
@@ -3428,10 +3461,10 @@
       <c r="C130" s="12"/>
       <c r="E130" s="11"/>
       <c r="I130" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J130" s="2" t="s">
-        <v>214</v>
+        <v>78</v>
       </c>
       <c r="K130">
         <v>1</v>
@@ -3440,357 +3473,385 @@
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C131" s="12"/>
-      <c r="E131" s="7" t="s">
+      <c r="E131" s="11"/>
+      <c r="I131" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="J131" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="K131">
+        <v>1</v>
+      </c>
+      <c r="R131" s="31"/>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C132" s="12"/>
+      <c r="E132" s="11"/>
+      <c r="I132" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="J132" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="K132">
+        <v>1</v>
+      </c>
+      <c r="R132" s="31"/>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C133" s="12"/>
+      <c r="E133" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I131" s="2" t="s">
+      <c r="I133" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="J131" s="2" t="s">
+      <c r="J133" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="K131">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C132" s="12" t="s">
+      <c r="K133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C134" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E132" s="5" t="s">
+      <c r="E134" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J132" s="2" t="s">
+      <c r="J134" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N132">
+      <c r="N134">
         <v>-4</v>
       </c>
-      <c r="P132" s="19"/>
-      <c r="Q132" s="31">
+      <c r="P134" s="19"/>
+      <c r="Q134" s="31">
         <v>0.3</v>
       </c>
-      <c r="R132" s="31"/>
-    </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C133" s="7"/>
-      <c r="E133" s="7" t="s">
+      <c r="R134" s="31"/>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C135" s="7"/>
+      <c r="E135" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="J133" s="2" t="s">
+      <c r="J135" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="N133">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C135" s="5" t="s">
+      <c r="N135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C137" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E135" s="5"/>
-      <c r="P135" s="31">
+      <c r="E137" s="5"/>
+      <c r="P137" s="31">
         <v>2</v>
       </c>
-      <c r="Q135" s="31"/>
-    </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C136" s="12" t="s">
+      <c r="Q137" s="31"/>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C138" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E136" s="11"/>
-      <c r="K136" s="32">
+      <c r="E138" s="11"/>
+      <c r="K138" s="32">
         <f>-80+8-14-6</f>
         <v>-92</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C137" s="27" t="s">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C139" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D137" s="35"/>
-      <c r="E137" s="28" t="s">
+      <c r="D139" s="33"/>
+      <c r="E139" s="28" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C138" s="12" t="s">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C140" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E138" s="11"/>
-      <c r="N138">
+      <c r="E140" s="11"/>
+      <c r="N140">
         <v>-1</v>
       </c>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C139" s="7" t="s">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C141" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E139" s="7" t="s">
+      <c r="E141" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="140" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C141" s="5" t="s">
+    <row r="142" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C143" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E141" s="5"/>
-    </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A142"/>
-      <c r="C142" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E142" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="I142" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="L142">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A143"/>
-      <c r="C143" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E143" s="37"/>
-      <c r="I143" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="K143">
-        <v>2</v>
-      </c>
+      <c r="E143" s="5"/>
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144"/>
       <c r="C144" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E144" s="37"/>
+        <v>54</v>
+      </c>
+      <c r="E144" s="37" t="s">
+        <v>227</v>
+      </c>
       <c r="I144" s="2" t="s">
-        <v>235</v>
+        <v>228</v>
+      </c>
+      <c r="L144">
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A145"/>
       <c r="C145" s="12" t="s">
-        <v>229</v>
+        <v>55</v>
       </c>
       <c r="E145" s="37"/>
+      <c r="I145" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="K145">
+        <v>2</v>
+      </c>
     </row>
     <row r="146" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A146"/>
-      <c r="C146" s="7" t="s">
+      <c r="C146" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E146" s="37"/>
+      <c r="I146" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="147" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A147"/>
+      <c r="C147" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="E147" s="37"/>
+    </row>
+    <row r="148" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A148"/>
+      <c r="C148" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E146" s="7" t="s">
+      <c r="E148" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I146" s="2" t="s">
+      <c r="I148" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="J146" s="2" t="s">
+      <c r="J148" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K146">
-        <v>1</v>
-      </c>
-      <c r="P146" s="19"/>
-      <c r="Q146" s="19"/>
-      <c r="R146" s="19"/>
-      <c r="T146" s="19">
+      <c r="K148">
+        <v>1</v>
+      </c>
+      <c r="P148" s="19"/>
+      <c r="Q148" s="19"/>
+      <c r="R148" s="19"/>
+      <c r="T148" s="19">
         <v>0.1</v>
       </c>
     </row>
-    <row r="147" spans="1:22" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A148" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C148" s="5" t="s">
+    <row r="149" spans="1:22" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C150" s="5" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="149" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A149"/>
-      <c r="C149" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E149" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="P149" s="9">
-        <v>-3</v>
-      </c>
-      <c r="S149" s="9">
-        <f>-P149/2</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="150" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A150"/>
-      <c r="C150" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E150" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q150" s="9">
-        <v>-3</v>
-      </c>
-      <c r="S150" s="9">
-        <f>-Q150/2</f>
-        <v>1.5</v>
       </c>
     </row>
     <row r="151" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A151"/>
       <c r="C151" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E151" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="R151" s="9">
+      <c r="P151" s="9">
         <v>-3</v>
       </c>
       <c r="S151" s="9">
-        <f>-R151/2</f>
+        <f>-P151/2</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="152" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A152"/>
-      <c r="C152" s="7" t="s">
+      <c r="C152" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E152" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q152" s="9">
+        <v>-3</v>
+      </c>
+      <c r="S152" s="9">
+        <f>-Q152/2</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A153"/>
+      <c r="C153" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E153" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="R153" s="9">
+        <v>-3</v>
+      </c>
+      <c r="S153" s="9">
+        <f>-R153/2</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A154"/>
+      <c r="C154" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E152" s="24" t="s">
+      <c r="E154" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="T152" s="9">
+      <c r="T154" s="9">
         <v>-6</v>
       </c>
-      <c r="U152" s="9">
-        <f>-T152/2</f>
+      <c r="U154" s="9">
+        <f>-T154/2</f>
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:22" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A154" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C154" s="5" t="s">
+    <row r="155" spans="1:22" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C156" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="155" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C155" s="12" t="s">
+    <row r="157" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C157" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E155" s="24" t="s">
+      <c r="E157" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="S155" s="25">
+      <c r="S157" s="25">
         <v>-40</v>
       </c>
-      <c r="U155" s="25"/>
-      <c r="V155" s="25"/>
-    </row>
-    <row r="156" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C156" s="12" t="s">
+      <c r="U157" s="25"/>
+      <c r="V157" s="25"/>
+    </row>
+    <row r="158" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C158" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E156" s="24" t="s">
+      <c r="E158" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="S156" s="25"/>
-      <c r="U156" s="25">
+      <c r="S158" s="25"/>
+      <c r="U158" s="25">
         <v>-40</v>
       </c>
-      <c r="V156" s="25"/>
-    </row>
-    <row r="157" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C157" s="7" t="s">
+      <c r="V158" s="25"/>
+    </row>
+    <row r="159" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C159" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E157" s="24" t="s">
+      <c r="E159" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="S157" s="25"/>
-      <c r="U157" s="25"/>
-      <c r="V157" s="25">
+      <c r="S159" s="25"/>
+      <c r="U159" s="25"/>
+      <c r="V159" s="25">
         <v>-40</v>
       </c>
     </row>
-    <row r="159" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C159" s="20" t="s">
+    <row r="161" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C161" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="D159" s="21"/>
-      <c r="E159" s="21"/>
-      <c r="F159" s="21"/>
-      <c r="G159" s="21"/>
-      <c r="H159" s="21"/>
-      <c r="I159" s="21"/>
-      <c r="J159" s="21"/>
-      <c r="K159" s="22">
-        <f>SUM(K2:K158)</f>
-        <v>-11</v>
-      </c>
-      <c r="L159" s="22">
-        <f>SUM(L2:L158)</f>
+      <c r="D161" s="21"/>
+      <c r="E161" s="21"/>
+      <c r="F161" s="21"/>
+      <c r="G161" s="21"/>
+      <c r="H161" s="21"/>
+      <c r="I161" s="21"/>
+      <c r="J161" s="21"/>
+      <c r="K161" s="22">
+        <f>SUM(K2:K160)</f>
+        <v>-9</v>
+      </c>
+      <c r="L161" s="22">
+        <f>SUM(L2:L160)</f>
         <v>0</v>
       </c>
-      <c r="M159" s="22">
-        <f>SUM(M2:M158)</f>
+      <c r="M161" s="22">
+        <f>SUM(M2:M160)</f>
         <v>0</v>
       </c>
-      <c r="N159" s="22">
-        <f>SUM(N2:N158)</f>
+      <c r="N161" s="22">
+        <f>SUM(N2:N160)</f>
         <v>0</v>
       </c>
-      <c r="O159" s="22"/>
-      <c r="P159" s="22">
-        <f>SUM(P2:P158)</f>
+      <c r="O161" s="22"/>
+      <c r="P161" s="22">
+        <f t="shared" ref="P161:V161" si="0">SUM(P2:P160)</f>
         <v>-1</v>
       </c>
-      <c r="Q159" s="22">
-        <f>SUM(Q2:Q158)</f>
+      <c r="Q161" s="22">
+        <f t="shared" si="0"/>
         <v>-2.2999999999999998</v>
       </c>
-      <c r="R159" s="22">
-        <f>SUM(R2:R158)</f>
+      <c r="R161" s="22">
+        <f t="shared" si="0"/>
         <v>-3.8000000000000256E-2</v>
       </c>
-      <c r="S159" s="22">
-        <f>SUM(S2:S158)</f>
-        <v>-35.5</v>
-      </c>
-      <c r="T159" s="22">
-        <f>SUM(T2:T158)</f>
+      <c r="S161" s="22">
+        <f t="shared" si="0"/>
+        <v>-35</v>
+      </c>
+      <c r="T161" s="22">
+        <f t="shared" si="0"/>
         <v>-1.6400000000000006</v>
       </c>
-      <c r="U159" s="22">
-        <f>SUM(U2:U158)</f>
+      <c r="U161" s="22">
+        <f t="shared" si="0"/>
         <v>-4.8999999999999986</v>
       </c>
-      <c r="V159" s="23">
-        <f>SUM(V2:V158)</f>
+      <c r="V161" s="23">
+        <f t="shared" si="0"/>
         <v>-20</v>
       </c>
     </row>
@@ -3798,7 +3859,7 @@
   <mergeCells count="3">
     <mergeCell ref="C45:C46"/>
     <mergeCell ref="C52:C53"/>
-    <mergeCell ref="E142:E145"/>
+    <mergeCell ref="E144:E147"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout de commentaires bug carte électronique sur le schéma
</commit_message>
<xml_diff>
--- a/hardware/expansion_board_V0/Conception.xlsx
+++ b/hardware/expansion_board_V0/Conception.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Robot_master\hardware\expansion_board_V0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Robot\hardware\expansion_board_V0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8625" yWindow="0" windowWidth="27705" windowHeight="13020"/>
+    <workbookView xWindow="9585" yWindow="0" windowWidth="27705" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -395,9 +395,6 @@
     <t>M1_PWMB</t>
   </si>
   <si>
-    <t>M1_FAULT</t>
-  </si>
-  <si>
     <t>M1_CS</t>
   </si>
   <si>
@@ -407,9 +404,6 @@
     <t>M0_PWMB</t>
   </si>
   <si>
-    <t>M0_FAULT</t>
-  </si>
-  <si>
     <t>M0_CS</t>
   </si>
   <si>
@@ -425,9 +419,6 @@
     <t>M3_PWMB</t>
   </si>
   <si>
-    <t>M23_FAULT</t>
-  </si>
-  <si>
     <t>M2_CS</t>
   </si>
   <si>
@@ -446,9 +437,6 @@
     <t>M5_PWMB</t>
   </si>
   <si>
-    <t>M45_FAULT</t>
-  </si>
-  <si>
     <t>QEI0_A</t>
   </si>
   <si>
@@ -641,9 +629,6 @@
     <t>Tension servo (A5V)</t>
   </si>
   <si>
-    <t>M4_CS</t>
-  </si>
-  <si>
     <t>M5 - Moteur (without CS)</t>
   </si>
   <si>
@@ -1005,6 +990,21 @@
   </si>
   <si>
     <t>QEI</t>
+  </si>
+  <si>
+    <t>M01_FAULT</t>
+  </si>
+  <si>
+    <t>M01_RESET</t>
+  </si>
+  <si>
+    <t>M23454_FAULT</t>
+  </si>
+  <si>
+    <t>M2345_RESET</t>
+  </si>
+  <si>
+    <t>M5_CS</t>
   </si>
 </sst>
 </file>
@@ -1294,15 +1294,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1591,7 +1591,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S131" sqref="S131"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,13 +1675,13 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1699,13 +1699,13 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -1727,13 +1727,13 @@
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>127</v>
+        <v>322</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -1756,10 +1756,10 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>22</v>
@@ -1793,13 +1793,13 @@
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>121</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -1816,13 +1816,13 @@
         <v>3</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>122</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -1835,13 +1835,13 @@
         <v>4</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>123</v>
+        <v>323</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -1858,10 +1858,10 @@
         <v>5</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>22</v>
@@ -1883,13 +1883,13 @@
         <v>10</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -1904,13 +1904,13 @@
       </c>
       <c r="D14" s="11"/>
       <c r="G14" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1926,13 +1926,13 @@
       <c r="C16" s="30"/>
       <c r="D16" s="11"/>
       <c r="G16" s="2" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1949,13 +1949,13 @@
         <v>63</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -1970,13 +1970,13 @@
         <v>12</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -1992,20 +1992,20 @@
       <c r="B20" s="12"/>
       <c r="D20" s="12"/>
       <c r="G20" s="2" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="8"/>
@@ -2013,13 +2013,13 @@
         <v>3</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -2040,13 +2040,13 @@
         <v>4</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -2058,13 +2058,13 @@
         <v>5</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>133</v>
+        <v>324</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -2076,10 +2076,10 @@
         <v>4</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>22</v>
@@ -2099,10 +2099,10 @@
         <v>5</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>22</v>
@@ -2123,13 +2123,13 @@
         <v>12</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -2145,30 +2145,30 @@
       <c r="B28" s="12"/>
       <c r="D28" s="12"/>
       <c r="G28" s="2" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J28">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B29" s="37"/>
+      <c r="B29" s="35"/>
       <c r="C29" s="8"/>
       <c r="D29" s="12"/>
       <c r="G29" s="2" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -2182,20 +2182,20 @@
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -2207,13 +2207,13 @@
         <v>4</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>140</v>
+        <v>325</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -2225,10 +2225,10 @@
         <v>5</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>205</v>
+        <v>326</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>22</v>
@@ -2247,13 +2247,13 @@
         <v>9</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -2266,13 +2266,13 @@
       <c r="B35" s="11"/>
       <c r="D35" s="11"/>
       <c r="G35" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="J35">
         <v>1</v>
@@ -2284,13 +2284,13 @@
       </c>
       <c r="D36" s="11"/>
       <c r="G36" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="J36">
         <v>1</v>
@@ -2303,13 +2303,13 @@
       <c r="C37" s="30"/>
       <c r="D37" s="11"/>
       <c r="G37" s="2" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="J37">
         <v>1</v>
@@ -2322,13 +2322,13 @@
       <c r="B38" s="11"/>
       <c r="D38" s="11"/>
       <c r="G38" s="2" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="J38">
         <v>1</v>
@@ -2342,13 +2342,13 @@
         <v>63</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="J39">
         <v>1</v>
@@ -2366,13 +2366,13 @@
         <v>18</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J41">
         <v>1</v>
@@ -2396,10 +2396,10 @@
         <v>16</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>0</v>
@@ -2418,17 +2418,17 @@
       </c>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="37" t="s">
         <v>19</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>22</v>
@@ -2441,7 +2441,7 @@
       </c>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B46" s="36"/>
+      <c r="B46" s="38"/>
       <c r="D46" s="7" t="s">
         <v>5</v>
       </c>
@@ -2456,13 +2456,13 @@
         <v>18</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J48">
         <v>1</v>
@@ -2486,10 +2486,10 @@
         <v>16</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>0</v>
@@ -2511,17 +2511,17 @@
       </c>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B52" s="35" t="s">
+      <c r="B52" s="37" t="s">
         <v>19</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>22</v>
@@ -2534,7 +2534,7 @@
       </c>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B53" s="36"/>
+      <c r="B53" s="38"/>
       <c r="D53" s="7" t="s">
         <v>5</v>
       </c>
@@ -2548,13 +2548,13 @@
         <v>9</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J55">
         <v>1</v>
@@ -2569,13 +2569,13 @@
       </c>
       <c r="D56" s="11"/>
       <c r="G56" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J56">
         <v>1</v>
@@ -2590,13 +2590,13 @@
       </c>
       <c r="D57" s="14"/>
       <c r="G57" s="2" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J57">
         <v>1</v>
@@ -2611,13 +2611,13 @@
       </c>
       <c r="D58" s="11"/>
       <c r="G58" s="2" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J58">
         <v>1</v>
@@ -2632,13 +2632,13 @@
       </c>
       <c r="D59" s="11"/>
       <c r="G59" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J59">
         <v>1</v>
@@ -2653,13 +2653,13 @@
       </c>
       <c r="D60" s="11"/>
       <c r="G60" s="2" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>105</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J60">
         <v>1</v>
@@ -2674,13 +2674,13 @@
       </c>
       <c r="D61" s="14"/>
       <c r="G61" s="2" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>106</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J61">
         <v>1</v>
@@ -2697,13 +2697,13 @@
         <v>63</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>107</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J62">
         <v>1</v>
@@ -2718,10 +2718,10 @@
         <v>4</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>22</v>
@@ -2734,10 +2734,10 @@
       <c r="B64" s="11"/>
       <c r="D64" s="11"/>
       <c r="G64" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>22</v>
@@ -2752,10 +2752,10 @@
       <c r="C65" s="1"/>
       <c r="D65" s="14"/>
       <c r="G65" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>22</v>
@@ -2770,10 +2770,10 @@
       <c r="C66" s="1"/>
       <c r="D66" s="11"/>
       <c r="G66" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>22</v>
@@ -2788,10 +2788,10 @@
       <c r="C67" s="1"/>
       <c r="D67" s="11"/>
       <c r="G67" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>22</v>
@@ -2806,10 +2806,10 @@
       <c r="C68" s="1"/>
       <c r="D68" s="11"/>
       <c r="G68" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>22</v>
@@ -2824,10 +2824,10 @@
       <c r="C69" s="1"/>
       <c r="D69" s="14"/>
       <c r="G69" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="I69" s="2" t="s">
         <v>22</v>
@@ -2838,14 +2838,14 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70"/>
-      <c r="B70" s="37"/>
+      <c r="B70" s="35"/>
       <c r="C70" s="1"/>
       <c r="D70" s="7"/>
       <c r="G70" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>22</v>
@@ -2863,10 +2863,10 @@
         <v>9</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>21</v>
@@ -2884,10 +2884,10 @@
       </c>
       <c r="D73" s="11"/>
       <c r="G73" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="I73" s="2" t="s">
         <v>21</v>
@@ -2905,7 +2905,7 @@
       </c>
       <c r="D74" s="14"/>
       <c r="G74" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>94</v>
@@ -2926,7 +2926,7 @@
       </c>
       <c r="D75" s="14"/>
       <c r="G75" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>95</v>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="D76" s="14"/>
       <c r="G76" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>96</v>
@@ -2968,7 +2968,7 @@
       </c>
       <c r="D77" s="11"/>
       <c r="G77" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>97</v>
@@ -2989,7 +2989,7 @@
       </c>
       <c r="D78" s="14"/>
       <c r="G78" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>98</v>
@@ -3012,7 +3012,7 @@
         <v>63</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>99</v>
@@ -3033,7 +3033,7 @@
         <v>84</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>84</v>
@@ -3053,7 +3053,7 @@
         <v>85</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>85</v>
@@ -3073,7 +3073,7 @@
         <v>86</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>86</v>
@@ -3093,7 +3093,7 @@
         <v>87</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>87</v>
@@ -3113,7 +3113,7 @@
         <v>88</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>88</v>
@@ -3133,7 +3133,7 @@
         <v>89</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>89</v>
@@ -3153,7 +3153,7 @@
         <v>90</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>90</v>
@@ -3173,7 +3173,7 @@
         <v>91</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>91</v>
@@ -3197,13 +3197,13 @@
         <v>9</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="J90">
         <v>1</v>
@@ -3216,13 +3216,13 @@
       <c r="B91" s="13"/>
       <c r="D91" s="12"/>
       <c r="G91" s="2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="J91">
         <v>1</v>
@@ -3234,13 +3234,13 @@
       </c>
       <c r="D92" s="11"/>
       <c r="G92" s="2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="J92">
         <v>1</v>
@@ -3253,13 +3253,13 @@
       <c r="B93" s="13"/>
       <c r="D93" s="11"/>
       <c r="G93" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="J93">
         <v>1</v>
@@ -3271,13 +3271,13 @@
       </c>
       <c r="D94" s="11"/>
       <c r="G94" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="J94">
         <v>1</v>
@@ -3290,13 +3290,13 @@
       <c r="B95" s="11"/>
       <c r="D95" s="11"/>
       <c r="G95" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="J95">
         <v>1</v>
@@ -3308,13 +3308,13 @@
       </c>
       <c r="D96" s="11"/>
       <c r="G96" s="2" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J96">
         <v>1</v>
@@ -3322,17 +3322,17 @@
     </row>
     <row r="97" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D97" s="11"/>
       <c r="G97" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="J97">
         <v>1</v>
@@ -3345,13 +3345,13 @@
       <c r="B98" s="11"/>
       <c r="D98" s="11"/>
       <c r="G98" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="J98">
         <v>1</v>
@@ -3359,19 +3359,19 @@
     </row>
     <row r="99" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B99" s="7" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>63</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="J99">
         <v>1</v>
@@ -3386,13 +3386,13 @@
         <v>9</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="J101">
         <v>1</v>
@@ -3405,13 +3405,13 @@
       <c r="B102" s="11"/>
       <c r="D102" s="11"/>
       <c r="G102" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="J102">
         <v>1</v>
@@ -3423,10 +3423,10 @@
       </c>
       <c r="D103" s="11"/>
       <c r="G103" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="I103" s="2" t="s">
         <v>0</v>
@@ -3441,13 +3441,13 @@
       </c>
       <c r="D104" s="11"/>
       <c r="G104" s="2" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="J104">
         <v>1</v>
@@ -3460,13 +3460,13 @@
       <c r="B105" s="11"/>
       <c r="D105" s="11"/>
       <c r="G105" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="J105">
         <v>1</v>
@@ -3477,13 +3477,13 @@
         <v>28</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>0</v>
@@ -3501,13 +3501,13 @@
         <v>9</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I108" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J108">
         <v>1</v>
@@ -3520,13 +3520,13 @@
       <c r="B109" s="11"/>
       <c r="D109" s="11"/>
       <c r="G109" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J109">
         <v>1</v>
@@ -3536,13 +3536,13 @@
       <c r="B110" s="11"/>
       <c r="D110" s="11"/>
       <c r="G110" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I110" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J110">
         <v>1</v>
@@ -3552,10 +3552,10 @@
       <c r="B111" s="11"/>
       <c r="D111" s="11"/>
       <c r="G111" s="2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I111" s="2" t="s">
         <v>29</v>
@@ -3570,13 +3570,13 @@
       </c>
       <c r="D112" s="11"/>
       <c r="G112" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J112">
         <v>1</v>
@@ -3589,13 +3589,13 @@
       <c r="B113" s="11"/>
       <c r="D113" s="11"/>
       <c r="G113" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J113">
         <v>1</v>
@@ -3605,13 +3605,13 @@
       <c r="B114" s="11"/>
       <c r="D114" s="11"/>
       <c r="G114" s="2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="I114" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J114">
         <v>1</v>
@@ -3623,10 +3623,10 @@
         <v>63</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="I115" s="2" t="s">
         <v>0</v>
@@ -3637,14 +3637,14 @@
     </row>
     <row r="116" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B116" s="11" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D116" s="11"/>
       <c r="G116" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="I116" s="2" t="s">
         <v>0</v>
@@ -3657,13 +3657,13 @@
       <c r="B117" s="11"/>
       <c r="D117" s="11"/>
       <c r="G117" s="2" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I117" s="2" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="J117">
         <v>1</v>
@@ -3672,13 +3672,13 @@
     <row r="118" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B118" s="13"/>
       <c r="D118" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I118" s="2" t="s">
         <v>0</v>
@@ -3690,7 +3690,7 @@
     <row r="119" spans="2:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="120" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B120" s="5" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D120" s="4"/>
     </row>
@@ -3702,13 +3702,13 @@
         <v>60</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="I121" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J121">
         <v>1</v>
@@ -3724,13 +3724,13 @@
       <c r="B122" s="12"/>
       <c r="D122" s="11"/>
       <c r="G122" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I122" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J122">
         <v>1</v>
@@ -3741,13 +3741,13 @@
       <c r="B123" s="12"/>
       <c r="D123" s="11"/>
       <c r="G123" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="I123" s="2" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="J123">
         <v>1</v>
@@ -3758,10 +3758,10 @@
       <c r="B124" s="12"/>
       <c r="D124" s="11"/>
       <c r="G124" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="I124" s="2" t="s">
         <v>0</v>
@@ -3777,13 +3777,13 @@
         <v>61</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="I125" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="J125">
         <v>1</v>
@@ -3797,13 +3797,13 @@
         <v>23</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I126" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J126">
         <v>1</v>
@@ -3819,13 +3819,13 @@
       <c r="B127" s="12"/>
       <c r="D127" s="11"/>
       <c r="G127" s="2" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="I127" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J127">
         <v>1</v>
@@ -3836,13 +3836,13 @@
       <c r="B128" s="12"/>
       <c r="D128" s="11"/>
       <c r="G128" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="H128" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="I128" s="2" t="s">
         <v>316</v>
-      </c>
-      <c r="H128" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="I128" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="J128">
         <v>1</v>
@@ -3853,10 +3853,10 @@
       <c r="B129" s="12"/>
       <c r="D129" s="11"/>
       <c r="G129" s="2" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I129" s="2" t="s">
         <v>0</v>
@@ -3870,13 +3870,13 @@
       <c r="B130" s="12"/>
       <c r="D130" s="11"/>
       <c r="G130" s="2" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I130" s="2" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="J130">
         <v>1</v>
@@ -3889,10 +3889,10 @@
         <v>24</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="I131" s="2" t="s">
         <v>0</v>
@@ -3913,7 +3913,7 @@
         <v>64</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="N133" s="19"/>
       <c r="O133" s="31">
@@ -3929,7 +3929,7 @@
         <v>64</v>
       </c>
       <c r="G134" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="O134" s="31">
         <v>0.4</v>
@@ -3942,7 +3942,7 @@
       </c>
       <c r="D135" s="15"/>
       <c r="G135" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="P135" s="9">
         <v>0.3</v>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="D136" s="15"/>
       <c r="G136" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="P136" s="9">
         <v>0.3</v>
@@ -3966,7 +3966,7 @@
       </c>
       <c r="D137" s="15"/>
       <c r="G137" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="138" spans="2:20" x14ac:dyDescent="0.25">
@@ -3977,7 +3977,7 @@
         <v>32</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="I138" s="2" t="s">
         <v>35</v>
@@ -3994,7 +3994,7 @@
         <v>31</v>
       </c>
       <c r="G139" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="I139" s="2" t="s">
         <v>36</v>
@@ -4003,19 +4003,19 @@
     <row r="140" spans="2:20" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="141" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B141" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="142" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B142" s="12" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D142" s="24"/>
       <c r="G142" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="I142" s="2" t="s">
         <v>0</v>
@@ -4029,14 +4029,14 @@
     </row>
     <row r="143" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B143" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D143" s="24"/>
       <c r="G143" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="I143" s="2" t="s">
         <v>0</v>
@@ -4104,13 +4104,13 @@
         <v>47</v>
       </c>
       <c r="D152" s="39" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H152" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I152" s="2" t="s">
         <v>22</v>
@@ -4125,10 +4125,10 @@
       </c>
       <c r="D153" s="39"/>
       <c r="G153" s="2" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I153" s="2" t="s">
         <v>0</v>
@@ -4143,10 +4143,10 @@
       </c>
       <c r="D154" s="39"/>
       <c r="G154" s="2" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I154" s="2" t="s">
         <v>0</v>
@@ -4157,7 +4157,7 @@
     </row>
     <row r="155" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B155" s="12" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D155" s="39"/>
     </row>
@@ -4169,10 +4169,10 @@
         <v>51</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="I156" s="2" t="s">
         <v>0</v>

</xml_diff>